<commit_message>
Those files belongs to one-table-My-SQL-connection. The primary key is the Search ID
</commit_message>
<xml_diff>
--- a/Web_Scraping_ML/Ofertas_MX/CSV_Design.xlsx
+++ b/Web_Scraping_ML/Ofertas_MX/CSV_Design.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisc\Desktop\WS_ML_MX\Ofertas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisc\Desktop\Web_Scrapers\Web_Scraping_ML\Ofertas_MX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACACFEE-3B6B-43FD-8D70-6C627C4C3692}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2E386D4-ABCC-41A9-8ADD-AB275AADA3A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -450,15 +451,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>

</xml_diff>